<commit_message>
update: 1. 新增 enum 规则
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -586,7 +586,7 @@
         <v/>
       </c>
       <c r="L5" t="str">
-        <v/>
+        <v>enum:10,11,12</v>
       </c>
     </row>
     <row r="6">
@@ -668,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="L7" t="str">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M7" t="str">
         <v>12</v>

</xml_diff>

<commit_message>
bugfix: 修复不生成 consts.json 的bug
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>__type__</t>
   </si>
@@ -67,6 +67,9 @@
     <t>enum:Weekday</t>
   </si>
   <si>
+    <t>array:map:int,string</t>
+  </si>
+  <si>
     <t>__name__</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t>weekday</t>
   </si>
   <si>
+    <t>nested</t>
+  </si>
+  <si>
     <t>__side__</t>
   </si>
   <si>
@@ -133,6 +139,9 @@
     <t>一个int类型值</t>
   </si>
   <si>
+    <t>嵌套类型</t>
+  </si>
+  <si>
     <t>__rule__</t>
   </si>
   <si>
@@ -199,7 +208,10 @@
     <t>Monday</t>
   </si>
   <si>
-    <t>"Hello Alpaca"</t>
+    <t>[{1:"Happy",2:"Smile"}]</t>
+  </si>
+  <si>
+    <t>"你好 Alpaca"</t>
   </si>
   <si>
     <t>{1:"nico",2:susu}</t>
@@ -209,6 +221,9 @@
   </si>
   <si>
     <t>Friday</t>
+  </si>
+  <si>
+    <t>[{-1:"开心",-2:"笑"}]</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1229,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -1229,9 +1244,10 @@
     <col min="14" max="14" width="18.125" customWidth="1"/>
     <col min="15" max="15" width="18.875" customWidth="1"/>
     <col min="17" max="17" width="14.125" customWidth="1"/>
+    <col min="18" max="18" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1283,245 +1299,263 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>33</v>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:17">
+    <row r="6" spans="2:18">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
+      <c r="Q6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="H6" t="s">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="K6" t="s">
+      <c r="H7" t="s">
         <v>55</v>
       </c>
-      <c r="L6" t="s">
+      <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="M6" t="s">
+      <c r="J7" t="s">
         <v>57</v>
       </c>
-      <c r="N6" t="s">
+      <c r="K7" t="s">
         <v>58</v>
       </c>
-      <c r="O6" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="L7" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>61</v>
       </c>
-      <c r="M7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" t="s">
-        <v>58</v>
-      </c>
       <c r="O7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="Q7" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="R7" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>